<commit_message>
Add one battle GUI per enemy
</commit_message>
<xml_diff>
--- a/home.xlsx
+++ b/home.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="L1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t xml:space="preserve">P</t>
   </si>
@@ -133,7 +133,7 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y23" activeCellId="0" sqref="Y23"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2084,7 +2084,7 @@
   </sheetPr>
   <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="X27" activeCellId="0" sqref="X27"/>
     </sheetView>
   </sheetViews>
@@ -7938,10 +7938,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7985,16 +7985,33 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expand and generalize enemy sprites/models
</commit_message>
<xml_diff>
--- a/home.xlsx
+++ b/home.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">T</t>
   </si>
   <si>
-    <t xml:space="preserve">E</t>
+    <t xml:space="preserve">S</t>
   </si>
 </sst>
 </file>
@@ -7941,7 +7941,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>